<commit_message>
modified:   JessicaCremonese_AM_Project.log 	modified:   JessicaCremonese_AM_Project.pdf 	modified:   JessicaCremonese_AM_Project.synctex.gz 	modified:   JessicaCremonese_AM_Project.tex 	new file:   Project_Code.asv 	modified:   Project_Code.m 	modified:   database_mpshocks_infoshocks.xlsx
</commit_message>
<xml_diff>
--- a/database_mpshocks_infoshocks.xlsx
+++ b/database_mpshocks_infoshocks.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\Applied Macro Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\AppMacro_Project_Efrem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4AD7C1-DE97-4DA5-B74D-CE814D008CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92451556-0295-4DA4-9F2E-493283EF2138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
+    <workbookView xWindow="8388" yWindow="1944" windowWidth="14652" windowHeight="9600" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Data Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -984,7 +984,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1017,6 +1017,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1042,7 +1048,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
@@ -1050,8 +1056,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal 6" xfId="2" xr:uid="{6242F30B-DEEF-4D49-AF4B-DF585DC2BC01}"/>
@@ -1388,35 +1393,35 @@
     <col min="12" max="12" width="143" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1634,7 +1639,7 @@
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10">

</xml_diff>

<commit_message>
modified:   JessicaCremonese_AM_Project.log 	modified:   JessicaCremonese_AM_Project.pdf 	modified:   JessicaCremonese_AM_Project.synctex.gz 	modified:   JessicaCremonese_AM_Project.tex 	modified:   Project_Code.m 	modified:   database_mpshocks_infoshocks.xlsx 	new file:   draft_MACRO PROJECT DEFINITIVE CODE.m 	new file:   draft_definitive_code_AM_efrem.asv 	new file:   draft_definitive_code_AM_efrem.m
</commit_message>
<xml_diff>
--- a/database_mpshocks_infoshocks.xlsx
+++ b/database_mpshocks_infoshocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\AppMacro_Project_Efrem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92451556-0295-4DA4-9F2E-493283EF2138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E41A4B8-2E86-4537-A162-E0790D6A367A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8388" yWindow="1944" windowWidth="14652" windowHeight="9600" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
   </bookViews>
@@ -723,18 +723,6 @@
     <t>2009m12</t>
   </si>
   <si>
-    <t>Unempl. Rate</t>
-  </si>
-  <si>
-    <t>3-month interest rate</t>
-  </si>
-  <si>
-    <t>10-yr-3-month spread</t>
-  </si>
-  <si>
-    <t>GFC new list (Miranda-Agrippino and Rey 2020 RESTUD)</t>
-  </si>
-  <si>
     <t>Data description</t>
   </si>
   <si>
@@ -969,10 +957,22 @@
     <t xml:space="preserve">MP_FF4, INFO_FF4: Miranda-Agrippino and Ricco's (2021 AEJM) monetary policy and info shocks (proxies)  </t>
   </si>
   <si>
-    <t>CPI core (less food and energy) index (US city average)</t>
-  </si>
-  <si>
     <t>Unempl. Rate, CPI, 3-month interest rate, 3-month interest rate: all downloaded from https://fred.stlouisfed.org/</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>GFC</t>
+  </si>
+  <si>
+    <t>Unempl_Rate</t>
+  </si>
+  <si>
+    <t>spread_10yr3month</t>
+  </si>
+  <si>
+    <t>interest_rate_3month</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544F8F59-4BE8-4B65-85A2-9A3D1352F03E}">
   <dimension ref="A1:Q302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,28 +1395,28 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>228</v>
+        <v>309</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>231</v>
+        <v>308</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -7580,7 +7580,7 @@
     </row>
     <row r="230" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B230">
         <v>1.1994444576297357E-2</v>
@@ -7607,7 +7607,7 @@
     </row>
     <row r="231" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -7634,7 +7634,7 @@
     </row>
     <row r="232" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B232">
         <v>-1.8650599338397481E-2</v>
@@ -7661,7 +7661,7 @@
     </row>
     <row r="233" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B233">
         <v>-1.702020124474736E-2</v>
@@ -7688,7 +7688,7 @@
     </row>
     <row r="234" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -7715,7 +7715,7 @@
     </row>
     <row r="235" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B235">
         <v>7.1662426822602073E-4</v>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="236" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -7769,7 +7769,7 @@
     </row>
     <row r="237" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B237">
         <v>-5.2941348833317262E-3</v>
@@ -7796,7 +7796,7 @@
     </row>
     <row r="238" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B238">
         <v>-8.3891614648813444E-3</v>
@@ -7823,7 +7823,7 @@
     </row>
     <row r="239" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -7850,7 +7850,7 @@
     </row>
     <row r="240" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B240">
         <v>-1.3199698224557015E-2</v>
@@ -7877,7 +7877,7 @@
     </row>
     <row r="241" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B241">
         <v>2.5543181768112543E-3</v>
@@ -7904,7 +7904,7 @@
     </row>
     <row r="242" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B242">
         <v>-3.0656089981524252E-2</v>
@@ -7931,7 +7931,7 @@
     </row>
     <row r="243" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -7958,7 +7958,7 @@
     </row>
     <row r="244" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B244">
         <v>-1.8585677896521102E-2</v>
@@ -7985,7 +7985,7 @@
     </row>
     <row r="245" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B245">
         <v>-1.4138760090350465E-2</v>
@@ -8012,7 +8012,7 @@
     </row>
     <row r="246" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -8039,7 +8039,7 @@
     </row>
     <row r="247" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B247">
         <v>-4.6047810621779291E-3</v>
@@ -8066,7 +8066,7 @@
     </row>
     <row r="248" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -8093,7 +8093,7 @@
     </row>
     <row r="249" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B249">
         <v>9.4258734618028715E-3</v>
@@ -8120,7 +8120,7 @@
     </row>
     <row r="250" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B250">
         <v>1.3756713899828073E-2</v>
@@ -8147,7 +8147,7 @@
     </row>
     <row r="251" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B251">
         <v>0</v>
@@ -8174,7 +8174,7 @@
     </row>
     <row r="252" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B252">
         <v>-5.5028104898054968E-3</v>
@@ -8201,7 +8201,7 @@
     </row>
     <row r="253" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B253">
         <v>-2.9205470239967338E-2</v>
@@ -8228,7 +8228,7 @@
     </row>
     <row r="254" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B254">
         <v>8.8362781005073276E-3</v>
@@ -8255,7 +8255,7 @@
     </row>
     <row r="255" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B255">
         <v>0</v>
@@ -8282,7 +8282,7 @@
     </row>
     <row r="256" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B256">
         <v>7.5974759995284698E-3</v>
@@ -8309,7 +8309,7 @@
     </row>
     <row r="257" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B257">
         <v>1.8357098408865725E-2</v>
@@ -8336,7 +8336,7 @@
     </row>
     <row r="258" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -8363,7 +8363,7 @@
     </row>
     <row r="259" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B259">
         <v>1.589185406089668E-2</v>
@@ -8390,7 +8390,7 @@
     </row>
     <row r="260" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -8417,7 +8417,7 @@
     </row>
     <row r="261" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B261">
         <v>1.661287192401615E-2</v>
@@ -8444,7 +8444,7 @@
     </row>
     <row r="262" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B262">
         <v>3.1242424386650515E-2</v>
@@ -8471,7 +8471,7 @@
     </row>
     <row r="263" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B263">
         <v>1.6179309510346726E-2</v>
@@ -8498,7 +8498,7 @@
     </row>
     <row r="264" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B264">
         <v>0</v>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="265" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B265">
         <v>1.7256235095771701E-2</v>
@@ -8552,7 +8552,7 @@
     </row>
     <row r="266" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B266">
         <v>1.1153930004877455E-2</v>
@@ -8579,7 +8579,7 @@
     </row>
     <row r="267" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B267">
         <v>0</v>
@@ -8606,7 +8606,7 @@
     </row>
     <row r="268" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B268">
         <v>2.6447902089091719E-2</v>
@@ -8633,7 +8633,7 @@
     </row>
     <row r="269" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B269">
         <v>0</v>
@@ -8660,7 +8660,7 @@
     </row>
     <row r="270" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B270">
         <v>3.0212176265493277E-2</v>
@@ -8687,7 +8687,7 @@
     </row>
     <row r="271" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B271">
         <v>2.0617573923858608E-2</v>
@@ -8714,7 +8714,7 @@
     </row>
     <row r="272" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B272">
         <v>2.6108121634076734E-3</v>
@@ -8741,7 +8741,7 @@
     </row>
     <row r="273" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -8768,7 +8768,7 @@
     </row>
     <row r="274" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B274">
         <v>1.7822548966521495E-2</v>
@@ -8795,7 +8795,7 @@
     </row>
     <row r="275" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B275">
         <v>6.793061429887135E-4</v>
@@ -8822,7 +8822,7 @@
     </row>
     <row r="276" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B276">
         <v>0</v>
@@ -8849,7 +8849,7 @@
     </row>
     <row r="277" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B277">
         <v>1.7991194872374536E-2</v>
@@ -8876,7 +8876,7 @@
     </row>
     <row r="278" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B278">
         <v>2.6381469688184406E-2</v>
@@ -8903,7 +8903,7 @@
     </row>
     <row r="279" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -8930,7 +8930,7 @@
     </row>
     <row r="280" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B280">
         <v>5.2215365585260697E-3</v>
@@ -8957,7 +8957,7 @@
     </row>
     <row r="281" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B281">
         <v>-1.1174776189933554E-2</v>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="282" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -9011,7 +9011,7 @@
     </row>
     <row r="283" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B283">
         <v>-7.4869318318125343E-3</v>
@@ -9038,7 +9038,7 @@
     </row>
     <row r="284" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B284">
         <v>-6.1278676682240199E-3</v>
@@ -9065,7 +9065,7 @@
     </row>
     <row r="285" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B285">
         <v>0</v>
@@ -9092,7 +9092,7 @@
     </row>
     <row r="286" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B286">
         <v>1.2994034095448886E-2</v>
@@ -9119,7 +9119,7 @@
     </row>
     <row r="287" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B287">
         <v>2.4516691526160577E-2</v>
@@ -9146,7 +9146,7 @@
     </row>
     <row r="288" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B288">
         <v>0</v>
@@ -9173,7 +9173,7 @@
     </row>
     <row r="289" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B289">
         <v>2.0315101982351775E-2</v>
@@ -9200,7 +9200,7 @@
     </row>
     <row r="290" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B290">
         <v>1.2165834037313429E-2</v>
@@ -9227,7 +9227,7 @@
     </row>
     <row r="291" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B291">
         <v>0</v>
@@ -9254,7 +9254,7 @@
     </row>
     <row r="292" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B292">
         <v>-1.1657296122197644E-2</v>
@@ -9281,7 +9281,7 @@
     </row>
     <row r="293" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B293">
         <v>-2.3146456591704285E-3</v>
@@ -9308,7 +9308,7 @@
     </row>
     <row r="294" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B294">
         <v>0</v>
@@ -9335,7 +9335,7 @@
     </row>
     <row r="295" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B295">
         <v>4.6784479858438073E-3</v>
@@ -9362,7 +9362,7 @@
     </row>
     <row r="296" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B296">
         <v>1.186267704812124E-2</v>
@@ -9389,7 +9389,7 @@
     </row>
     <row r="297" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B297">
         <v>0</v>
@@ -9416,7 +9416,7 @@
     </row>
     <row r="298" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B298">
         <v>-2.9973191247055171E-2</v>
@@ -9443,7 +9443,7 @@
     </row>
     <row r="299" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B299">
         <v>4.8470496656468104E-2</v>
@@ -9470,7 +9470,7 @@
     </row>
     <row r="300" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B300">
         <v>0</v>
@@ -9497,7 +9497,7 @@
     </row>
     <row r="301" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B301">
         <v>3.8523904682742215E-2</v>
@@ -9546,22 +9546,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new file:   Graphs/IRF 68 conf bands (lilla).svg 	new file:   Graphs/IRF 95 conf bands (lilla).svg 	new file:   Graphs/SerieStoricaVars.svg 	modified:   JessicaCremonese_AM_Project.aux 	modified:   JessicaCremonese_AM_Project.log 	modified:   JessicaCremonese_AM_Project.pdf 	modified:   JessicaCremonese_AM_Project.synctex.gz 	modified:   JessicaCremonese_AM_Project.tex 	deleted:    Project_Code.m 	modified:   database_mpshocks_infoshocks.xlsx 	deleted:    draft_MACRO PROJECT DEFINITIVE CODE.m 	deleted:    draft_definitive_code_AM_efrem.asv 	modified:   draft_definitive_code_AM_efrem.m
</commit_message>
<xml_diff>
--- a/database_mpshocks_infoshocks.xlsx
+++ b/database_mpshocks_infoshocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\AppMacro_Project_Efrem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E41A4B8-2E86-4537-A162-E0790D6A367A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB31C17-4140-40C9-B2AC-40CB3EE6EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8388" yWindow="1944" windowWidth="14652" windowHeight="9600" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -960,9 +960,6 @@
     <t>Unempl. Rate, CPI, 3-month interest rate, 3-month interest rate: all downloaded from https://fred.stlouisfed.org/</t>
   </si>
   <si>
-    <t>CPI</t>
-  </si>
-  <si>
     <t>GFC</t>
   </si>
   <si>
@@ -973,6 +970,9 @@
   </si>
   <si>
     <t>interest_rate_3month</t>
+  </si>
+  <si>
+    <t>logCPI100</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544F8F59-4BE8-4B65-85A2-9A3D1352F03E}">
   <dimension ref="A1:Q302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,19 +1404,19 @@
         <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1437,7 +1437,7 @@
         <v>6.4</v>
       </c>
       <c r="E2" s="6">
-        <v>139.5</v>
+        <v>214.45742076096161</v>
       </c>
       <c r="F2" s="4">
         <v>6.2228571428571433</v>
@@ -1463,7 +1463,7 @@
         <v>6.6</v>
       </c>
       <c r="E3" s="6">
-        <v>140.19999999999999</v>
+        <v>214.67480136306398</v>
       </c>
       <c r="F3" s="4">
         <v>5.9442105263157892</v>
@@ -1490,7 +1490,7 @@
         <v>6.8</v>
       </c>
       <c r="E4" s="6">
-        <v>140.5</v>
+        <v>214.76763242410985</v>
       </c>
       <c r="F4" s="4">
         <v>5.9050000000000002</v>
@@ -1517,7 +1517,7 @@
         <v>6.7</v>
       </c>
       <c r="E5" s="6">
-        <v>140.9</v>
+        <v>214.89109931093563</v>
       </c>
       <c r="F5" s="4">
         <v>5.6481818181818184</v>
@@ -1544,7 +1544,7 @@
         <v>6.9</v>
       </c>
       <c r="E6" s="6">
-        <v>141.30000000000001</v>
+        <v>215.01421618485588</v>
       </c>
       <c r="F6" s="4">
         <v>5.4609090909090909</v>
@@ -1571,7 +1571,7 @@
         <v>6.9</v>
       </c>
       <c r="E7" s="6">
-        <v>141.80000000000001</v>
+        <v>215.16762308470479</v>
       </c>
       <c r="F7" s="4">
         <v>5.5730000000000004</v>
@@ -1598,7 +1598,7 @@
         <v>6.8</v>
       </c>
       <c r="E8" s="6">
-        <v>142.30000000000001</v>
+        <v>215.32049000842846</v>
       </c>
       <c r="F8" s="4">
         <v>5.5750000000000002</v>
@@ -1625,7 +1625,7 @@
         <v>6.9</v>
       </c>
       <c r="E9" s="6">
-        <v>142.9</v>
+        <v>215.50322287909705</v>
       </c>
       <c r="F9" s="4">
         <v>5.333181818181818</v>
@@ -1652,7 +1652,7 @@
         <v>6.9</v>
       </c>
       <c r="E10" s="6">
-        <v>143.4</v>
+        <v>215.65491513317815</v>
       </c>
       <c r="F10" s="4">
         <v>5.2149999999999999</v>
@@ -1679,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="6">
-        <v>143.69999999999999</v>
+        <v>215.74567681342259</v>
       </c>
       <c r="F11" s="4">
         <v>4.9940909090909091</v>
@@ -1706,7 +1706,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="6">
-        <v>144.19999999999999</v>
+        <v>215.89652603834102</v>
       </c>
       <c r="F12" s="4">
         <v>4.5589473684210526</v>
@@ -1733,7 +1733,7 @@
         <v>7.3</v>
       </c>
       <c r="E13" s="6">
-        <v>144.69999999999999</v>
+        <v>216.04685311190374</v>
       </c>
       <c r="F13" s="4">
         <v>4.0738095238095235</v>
@@ -1760,7 +1760,7 @@
         <v>7.3</v>
       </c>
       <c r="E14" s="6">
-        <v>145.1</v>
+        <v>216.1667412437736</v>
       </c>
       <c r="F14" s="4">
         <v>3.804761904761905</v>
@@ -1787,7 +1787,7 @@
         <v>7.4</v>
       </c>
       <c r="E15" s="6">
-        <v>145.4</v>
+        <v>216.2564406523019</v>
       </c>
       <c r="F15" s="4">
         <v>3.8442105263157895</v>
@@ -1814,7 +1814,7 @@
         <v>7.4</v>
       </c>
       <c r="E16" s="6">
-        <v>145.9</v>
+        <v>216.40552918934515</v>
       </c>
       <c r="F16" s="4">
         <v>4.0359090909090911</v>
@@ -1841,7 +1841,7 @@
         <v>7.4</v>
       </c>
       <c r="E17" s="6">
-        <v>146.30000000000001</v>
+        <v>216.52443261253106</v>
       </c>
       <c r="F17" s="4">
         <v>3.749047619047619</v>
@@ -1868,7 +1868,7 @@
         <v>7.6</v>
       </c>
       <c r="E18" s="6">
-        <v>146.80000000000001</v>
+        <v>216.67260555800519</v>
       </c>
       <c r="F18" s="4">
         <v>3.633</v>
@@ -1895,7 +1895,7 @@
         <v>7.8</v>
       </c>
       <c r="E19" s="6">
-        <v>147.1</v>
+        <v>216.76126727275303</v>
       </c>
       <c r="F19" s="4">
         <v>3.6563636363636363</v>
@@ -1922,7 +1922,7 @@
         <v>7.7</v>
       </c>
       <c r="E20" s="6">
-        <v>147.6</v>
+        <v>216.90863574870227</v>
       </c>
       <c r="F20" s="4">
         <v>3.208181818181818</v>
@@ -1949,7 +1949,7 @@
         <v>7.6</v>
       </c>
       <c r="E21" s="6">
-        <v>147.9</v>
+        <v>216.99681739968923</v>
       </c>
       <c r="F21" s="4">
         <v>3.1271428571428572</v>
@@ -1976,7 +1976,7 @@
         <v>7.6</v>
       </c>
       <c r="E22" s="6">
-        <v>148.1</v>
+        <v>217.05550585212086</v>
       </c>
       <c r="F22" s="4">
         <v>2.9095238095238094</v>
@@ -2003,7 +2003,7 @@
         <v>7.3</v>
       </c>
       <c r="E23" s="6">
-        <v>148.80000000000001</v>
+        <v>217.26029312098598</v>
       </c>
       <c r="F23" s="4">
         <v>2.8638095238095236</v>
@@ -2030,7 +2030,7 @@
         <v>7.4</v>
       </c>
       <c r="E24" s="6">
-        <v>149.19999999999999</v>
+        <v>217.37688231366499</v>
       </c>
       <c r="F24" s="4">
         <v>3.128421052631579</v>
@@ -2057,7 +2057,7 @@
         <v>7.4</v>
       </c>
       <c r="E25" s="6">
-        <v>149.6</v>
+        <v>217.49315935284423</v>
       </c>
       <c r="F25" s="4">
         <v>3.2168181818181818</v>
@@ -2084,7 +2084,7 @@
         <v>7.3</v>
       </c>
       <c r="E26" s="6">
-        <v>150.1</v>
+        <v>217.63806922432701</v>
       </c>
       <c r="F26" s="4">
         <v>3.0015789473684209</v>
@@ -2111,7 +2111,7 @@
         <v>7.1</v>
       </c>
       <c r="E27" s="6">
-        <v>150.6</v>
+        <v>217.78249718646819</v>
       </c>
       <c r="F27" s="4">
         <v>2.9284210526315788</v>
@@ -2138,7 +2138,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="6">
-        <v>150.80000000000001</v>
+        <v>217.84013415337552</v>
       </c>
       <c r="F28" s="4">
         <v>2.9517391304347824</v>
@@ -2165,7 +2165,7 @@
         <v>7.1</v>
       </c>
       <c r="E29" s="6">
-        <v>151.4</v>
+        <v>218.0125875164054</v>
       </c>
       <c r="F29" s="4">
         <v>2.87</v>
@@ -2192,7 +2192,7 @@
         <v>7.1</v>
       </c>
       <c r="E30" s="6">
-        <v>151.80000000000001</v>
+        <v>218.12717715594613</v>
       </c>
       <c r="F30" s="4">
         <v>2.9565000000000001</v>
@@ -2219,7 +2219,7 @@
         <v>7</v>
       </c>
       <c r="E31" s="6">
-        <v>152.1</v>
+        <v>218.21292140529982</v>
       </c>
       <c r="F31" s="4">
         <v>3.0709090909090908</v>
@@ -2246,7 +2246,7 @@
         <v>6.9</v>
       </c>
       <c r="E32" s="6">
-        <v>152.30000000000001</v>
+        <v>218.26999033360428</v>
       </c>
       <c r="F32" s="4">
         <v>3.0361904761904763</v>
@@ -2273,7 +2273,7 @@
         <v>6.8</v>
       </c>
       <c r="E33" s="6">
-        <v>152.80000000000001</v>
+        <v>218.41233542396711</v>
       </c>
       <c r="F33" s="4">
         <v>3.019090909090909</v>
@@ -2300,7 +2300,7 @@
         <v>6.7</v>
       </c>
       <c r="E34" s="6">
-        <v>152.9</v>
+        <v>218.44074854123204</v>
       </c>
       <c r="F34" s="4">
         <v>2.9476190476190478</v>
@@ -2327,7 +2327,7 @@
         <v>6.8</v>
       </c>
       <c r="E35" s="6">
-        <v>153.4</v>
+        <v>218.5825359612962</v>
       </c>
       <c r="F35" s="4">
         <v>3.0175000000000001</v>
@@ -2354,7 +2354,7 @@
         <v>6.6</v>
       </c>
       <c r="E36" s="6">
-        <v>153.9</v>
+        <v>218.72386198314788</v>
       </c>
       <c r="F36" s="4">
         <v>3.1040000000000001</v>
@@ -2381,7 +2381,7 @@
         <v>6.5</v>
       </c>
       <c r="E37" s="6">
-        <v>154.30000000000001</v>
+        <v>218.83659260631484</v>
       </c>
       <c r="F37" s="4">
         <v>3.0568181818181817</v>
@@ -2408,7 +2408,7 @@
         <v>6.6</v>
       </c>
       <c r="E38" s="6">
-        <v>154.5</v>
+        <v>218.89284837608534</v>
       </c>
       <c r="F38" s="4">
         <v>2.9754999999999998</v>
@@ -2435,7 +2435,7 @@
         <v>6.6</v>
       </c>
       <c r="E39" s="6">
-        <v>154.80000000000001</v>
+        <v>218.9770956346874</v>
       </c>
       <c r="F39" s="4">
         <v>3.2536842105263157</v>
@@ -2462,7 +2462,7 @@
         <v>6.5</v>
       </c>
       <c r="E40" s="6">
-        <v>155.30000000000001</v>
+        <v>219.11714557285586</v>
       </c>
       <c r="F40" s="4">
         <v>3.5030434782608695</v>
@@ -2489,7 +2489,7 @@
         <v>6.4</v>
       </c>
       <c r="E41" s="6">
-        <v>155.5</v>
+        <v>219.17303933628563</v>
       </c>
       <c r="F41" s="4">
         <v>3.6784210526315788</v>
@@ -2516,7 +2516,7 @@
         <v>6.1</v>
       </c>
       <c r="E42" s="6">
-        <v>155.9</v>
+        <v>219.28461151888419</v>
       </c>
       <c r="F42" s="4">
         <v>4.1447619047619044</v>
@@ -2543,7 +2543,7 @@
         <v>6.1</v>
       </c>
       <c r="E43" s="6">
-        <v>156.4</v>
+        <v>219.42367487238292</v>
       </c>
       <c r="F43" s="4">
         <v>4.1368181818181817</v>
@@ -2570,7 +2570,7 @@
         <v>6.1</v>
       </c>
       <c r="E44" s="6">
-        <v>156.69999999999999</v>
+        <v>219.50689964685898</v>
       </c>
       <c r="F44" s="4">
         <v>4.3304999999999998</v>
@@ -2597,7 +2597,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="6">
-        <v>157.1</v>
+        <v>219.61761850399733</v>
       </c>
       <c r="F45" s="4">
         <v>4.4791304347826086</v>
@@ -2624,7 +2624,7 @@
         <v>5.9</v>
       </c>
       <c r="E46" s="6">
-        <v>157.5</v>
+        <v>219.72805581256191</v>
       </c>
       <c r="F46" s="4">
         <v>4.6247619047619049</v>
@@ -2651,7 +2651,7 @@
         <v>5.8</v>
       </c>
       <c r="E47" s="6">
-        <v>157.80000000000001</v>
+        <v>219.81069988734015</v>
       </c>
       <c r="F47" s="4">
         <v>4.9465000000000003</v>
@@ -2678,7 +2678,7 @@
         <v>5.6</v>
       </c>
       <c r="E48" s="6">
-        <v>158.19999999999999</v>
+        <v>219.92064791616576</v>
       </c>
       <c r="F48" s="4">
         <v>5.2889999999999997</v>
@@ -2705,7 +2705,7 @@
         <v>5.5</v>
       </c>
       <c r="E49" s="6">
-        <v>158.30000000000001</v>
+        <v>219.9480914862356</v>
       </c>
       <c r="F49" s="4">
         <v>5.5957142857142861</v>
@@ -2732,7 +2732,7 @@
         <v>5.6</v>
       </c>
       <c r="E50" s="6">
-        <v>159</v>
+        <v>220.13971243204514</v>
       </c>
       <c r="F50" s="4">
         <v>5.7104999999999997</v>
@@ -2759,7 +2759,7 @@
         <v>5.4</v>
       </c>
       <c r="E51" s="6">
-        <v>159.4</v>
+        <v>220.24883170600936</v>
       </c>
       <c r="F51" s="4">
         <v>5.7694736842105261</v>
@@ -2786,7 +2786,7 @@
         <v>5.4</v>
       </c>
       <c r="E52" s="6">
-        <v>159.9</v>
+        <v>220.38484637462346</v>
       </c>
       <c r="F52" s="4">
         <v>5.7286956521739132</v>
@@ -2813,7 +2813,7 @@
         <v>5.8</v>
       </c>
       <c r="E53" s="6">
-        <v>160.4</v>
+        <v>220.52043639481445</v>
       </c>
       <c r="F53" s="4">
         <v>5.6536842105263156</v>
@@ -2840,7 +2840,7 @@
         <v>5.6</v>
       </c>
       <c r="E54" s="6">
-        <v>160.69999999999999</v>
+        <v>220.60158767633445</v>
       </c>
       <c r="F54" s="4">
         <v>5.665</v>
@@ -2867,7 +2867,7 @@
         <v>5.6</v>
       </c>
       <c r="E55" s="6">
-        <v>161.1</v>
+        <v>220.70955404192182</v>
       </c>
       <c r="F55" s="4">
         <v>5.4722727272727276</v>
@@ -2894,7 +2894,7 @@
         <v>5.7</v>
       </c>
       <c r="E56" s="6">
-        <v>161.4</v>
+        <v>220.79035303860513</v>
       </c>
       <c r="F56" s="4">
         <v>5.4219999999999997</v>
@@ -2921,7 +2921,7 @@
         <v>5.7</v>
       </c>
       <c r="E57" s="6">
-        <v>161.80000000000001</v>
+        <v>220.89785172762535</v>
       </c>
       <c r="F57" s="4">
         <v>5.3978260869565213</v>
@@ -2948,7 +2948,7 @@
         <v>5.6</v>
       </c>
       <c r="E58" s="6">
-        <v>162.19999999999999</v>
+        <v>221.00508498751373</v>
       </c>
       <c r="F58" s="4">
         <v>5.2789999999999999</v>
@@ -2975,7 +2975,7 @@
         <v>5.5</v>
       </c>
       <c r="E59" s="6">
-        <v>162.69999999999999</v>
+        <v>221.13875529368588</v>
       </c>
       <c r="F59" s="4">
         <v>5.2785714285714285</v>
@@ -3002,7 +3002,7 @@
         <v>5.6</v>
       </c>
       <c r="E60" s="6">
-        <v>163</v>
+        <v>221.21876044039576</v>
       </c>
       <c r="F60" s="4">
         <v>5.3561904761904762</v>
@@ -3029,7 +3029,7 @@
         <v>5.6</v>
       </c>
       <c r="E61" s="6">
-        <v>163.1</v>
+        <v>221.24539610402758</v>
       </c>
       <c r="F61" s="4">
         <v>5.1435000000000004</v>
@@ -3056,7 +3056,7 @@
         <v>5.6</v>
       </c>
       <c r="E62" s="6">
-        <v>163.69999999999999</v>
+        <v>221.40486794119414</v>
       </c>
       <c r="F62" s="4">
         <v>4.996666666666667</v>
@@ -3083,7 +3083,7 @@
         <v>5.5</v>
       </c>
       <c r="E63" s="6">
-        <v>164</v>
+        <v>221.4843848047698</v>
       </c>
       <c r="F63" s="4">
         <v>4.8265000000000002</v>
@@ -3110,7 +3110,7 @@
         <v>5.5</v>
       </c>
       <c r="E64" s="6">
-        <v>164.4</v>
+        <v>221.59018132040319</v>
       </c>
       <c r="F64" s="4">
         <v>4.9623809523809523</v>
@@ -3137,7 +3137,7 @@
         <v>5.6</v>
       </c>
       <c r="E65" s="6">
-        <v>164.6</v>
+        <v>221.64298308762511</v>
       </c>
       <c r="F65" s="4">
         <v>4.9518181818181821</v>
@@ -3164,7 +3164,7 @@
         <v>5.6</v>
       </c>
       <c r="E66" s="6">
-        <v>165</v>
+        <v>221.74839442139063</v>
       </c>
       <c r="F66" s="4">
         <v>5.0154545454545456</v>
@@ -3191,7 +3191,7 @@
         <v>5.3</v>
       </c>
       <c r="E67" s="6">
-        <v>165.4</v>
+        <v>221.85355052165278</v>
       </c>
       <c r="F67" s="4">
         <v>5.0940000000000003</v>
@@ -3218,7 +3218,7 @@
         <v>5.5</v>
       </c>
       <c r="E68" s="6">
-        <v>165.7</v>
+        <v>221.93225084193369</v>
       </c>
       <c r="F68" s="4">
         <v>5.1504545454545454</v>
@@ -3245,7 +3245,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E69" s="6">
-        <v>166</v>
+        <v>222.01080880400551</v>
       </c>
       <c r="F69" s="4">
         <v>5.0468181818181819</v>
@@ -3272,7 +3272,7 @@
         <v>5.2</v>
       </c>
       <c r="E70" s="6">
-        <v>166.5</v>
+        <v>222.14142378423384</v>
       </c>
       <c r="F70" s="4">
         <v>5.0914999999999999</v>
@@ -3299,7 +3299,7 @@
         <v>5.2</v>
       </c>
       <c r="E71" s="6">
-        <v>166.8</v>
+        <v>222.219604630172</v>
       </c>
       <c r="F71" s="4">
         <v>4.9859090909090913</v>
@@ -3326,7 +3326,7 @@
         <v>5.4</v>
       </c>
       <c r="E72" s="6">
-        <v>167.2</v>
+        <v>222.32362731029974</v>
       </c>
       <c r="F72" s="4">
         <v>5.0284210526315789</v>
@@ -3353,7 +3353,7 @@
         <v>5.4</v>
       </c>
       <c r="E73" s="6">
-        <v>167.4</v>
+        <v>222.37554536572412</v>
       </c>
       <c r="F73" s="4">
         <v>4.9109523809523807</v>
@@ -3380,7 +3380,7 @@
         <v>5.3</v>
       </c>
       <c r="E74" s="6">
-        <v>167.8</v>
+        <v>222.47919564926818</v>
       </c>
       <c r="F74" s="4">
         <v>5.0338095238095235</v>
@@ -3407,7 +3407,7 @@
         <v>5.2</v>
       </c>
       <c r="E75" s="6">
-        <v>168.1</v>
+        <v>222.5567713439471</v>
       </c>
       <c r="F75" s="4">
         <v>5.0057894736842101</v>
@@ -3434,7 +3434,7 @@
         <v>5.2</v>
       </c>
       <c r="E76" s="6">
-        <v>168.4</v>
+        <v>222.63420871636308</v>
       </c>
       <c r="F76" s="4">
         <v>5.1440000000000001</v>
@@ -3461,7 +3461,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E77" s="6">
-        <v>168.9</v>
+        <v>222.76296495710088</v>
       </c>
       <c r="F77" s="4">
         <v>5.1622727272727271</v>
@@ -3488,7 +3488,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E78" s="6">
-        <v>169.2</v>
+        <v>222.84003587030048</v>
       </c>
       <c r="F78" s="4">
         <v>5.0480952380952377</v>
@@ -3515,7 +3515,7 @@
         <v>5</v>
       </c>
       <c r="E79" s="6">
-        <v>169.4</v>
+        <v>222.8913405994688</v>
       </c>
       <c r="F79" s="4">
         <v>4.9309523809523812</v>
@@ -3542,7 +3542,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E80" s="6">
-        <v>169.7</v>
+        <v>222.96818423176759</v>
       </c>
       <c r="F80" s="4">
         <v>5.0522727272727277</v>
@@ -3569,7 +3569,7 @@
         <v>4.8</v>
       </c>
       <c r="E81" s="6">
-        <v>169.8</v>
+        <v>222.99376859079339</v>
       </c>
       <c r="F81" s="4">
         <v>5.1419047619047618</v>
@@ -3596,7 +3596,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E82" s="6">
-        <v>170.2</v>
+        <v>223.09595557485687</v>
       </c>
       <c r="F82" s="4">
         <v>4.9528571428571428</v>
@@ -3623,7 +3623,7 @@
         <v>4.7</v>
       </c>
       <c r="E83" s="6">
-        <v>170.6</v>
+        <v>223.1979026831504</v>
       </c>
       <c r="F83" s="4">
         <v>4.9727272727272727</v>
@@ -3650,7 +3650,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E84" s="6">
-        <v>170.8</v>
+        <v>223.24878663529861</v>
       </c>
       <c r="F84" s="4">
         <v>5.1433333333333335</v>
@@ -3677,7 +3677,7 @@
         <v>4.7</v>
       </c>
       <c r="E85" s="6">
-        <v>171.2</v>
+        <v>223.35037603411342</v>
       </c>
       <c r="F85" s="4">
         <v>5.1622727272727271</v>
@@ -3704,7 +3704,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E86" s="6">
-        <v>171.6</v>
+        <v>223.45172835126866</v>
       </c>
       <c r="F86" s="4">
         <v>5.0369999999999999</v>
@@ -3731,7 +3731,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E87" s="6">
-        <v>171.9</v>
+        <v>223.52758766870525</v>
       </c>
       <c r="F87" s="4">
         <v>5.0857894736842102</v>
@@ -3758,7 +3758,7 @@
         <v>4.7</v>
       </c>
       <c r="E88" s="6">
-        <v>172.2</v>
+        <v>223.60331471176357</v>
       </c>
       <c r="F88" s="4">
         <v>5.0318181818181822</v>
@@ -3785,7 +3785,7 @@
         <v>4.3</v>
       </c>
       <c r="E89" s="6">
-        <v>172.5</v>
+        <v>223.67890994092926</v>
       </c>
       <c r="F89" s="4">
         <v>4.9495238095238099</v>
@@ -3812,7 +3812,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E90" s="6">
-        <v>172.9</v>
+        <v>223.77949932739227</v>
       </c>
       <c r="F90" s="4">
         <v>4.9984999999999999</v>
@@ -3839,7 +3839,7 @@
         <v>4.5</v>
       </c>
       <c r="E91" s="6">
-        <v>173.2</v>
+        <v>223.85478876813275</v>
       </c>
       <c r="F91" s="4">
         <v>4.9754545454545456</v>
@@ -3866,7 +3866,7 @@
         <v>4.5</v>
       </c>
       <c r="E92" s="6">
-        <v>173.5</v>
+        <v>223.92994791268924</v>
       </c>
       <c r="F92" s="4">
         <v>4.9636363636363638</v>
@@ -3893,7 +3893,7 @@
         <v>4.5</v>
       </c>
       <c r="E93" s="6">
-        <v>174</v>
+        <v>224.05492482826</v>
       </c>
       <c r="F93" s="4">
         <v>4.9023809523809527</v>
@@ -3920,7 +3920,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E94" s="6">
-        <v>174.2</v>
+        <v>224.10481506716442</v>
       </c>
       <c r="F94" s="4">
         <v>4.6061904761904762</v>
@@ -3947,7 +3947,7 @@
         <v>4.5</v>
       </c>
       <c r="E95" s="6">
-        <v>174.4</v>
+        <v>224.15464805965485</v>
       </c>
       <c r="F95" s="4">
         <v>3.9614285714285713</v>
@@ -3974,7 +3974,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E96" s="6">
-        <v>174.8</v>
+        <v>224.25414282983843</v>
       </c>
       <c r="F96" s="4">
         <v>4.4147368421052633</v>
@@ -4001,7 +4001,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E97" s="6">
-        <v>175.4</v>
+        <v>224.4029589030022</v>
       </c>
       <c r="F97" s="4">
         <v>4.3909090909090907</v>
@@ -4028,7 +4028,7 @@
         <v>4.3</v>
       </c>
       <c r="E98" s="6">
-        <v>175.6</v>
+        <v>224.45245115700837</v>
       </c>
       <c r="F98" s="4">
         <v>4.3352631578947367</v>
@@ -4055,7 +4055,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E99" s="6">
-        <v>175.6</v>
+        <v>224.45245115700837</v>
       </c>
       <c r="F99" s="4">
         <v>4.438421052631579</v>
@@ -4082,7 +4082,7 @@
         <v>4.2</v>
       </c>
       <c r="E100" s="6">
-        <v>175.7</v>
+        <v>224.4771761495295</v>
       </c>
       <c r="F100" s="4">
         <v>4.4408695652173913</v>
@@ -4109,7 +4109,7 @@
         <v>4.3</v>
       </c>
       <c r="E101" s="6">
-        <v>176.3</v>
+        <v>224.62523122993221</v>
       </c>
       <c r="F101" s="4">
         <v>4.2895454545454541</v>
@@ -4136,7 +4136,7 @@
         <v>4.2</v>
       </c>
       <c r="E102" s="6">
-        <v>176.5</v>
+        <v>224.67447097238414</v>
       </c>
       <c r="F102" s="4">
         <v>4.4984999999999999</v>
@@ -4163,7 +4163,7 @@
         <v>4.3</v>
       </c>
       <c r="E103" s="6">
-        <v>176.6</v>
+        <v>224.69906992415497</v>
       </c>
       <c r="F103" s="4">
         <v>4.5668181818181814</v>
@@ -4190,7 +4190,7 @@
         <v>4.3</v>
       </c>
       <c r="E104" s="6">
-        <v>177.1</v>
+        <v>224.82185611900749</v>
       </c>
       <c r="F104" s="4">
         <v>4.5509523809523813</v>
@@ -4217,7 +4217,7 @@
         <v>4.2</v>
       </c>
       <c r="E105" s="6">
-        <v>177.3</v>
+        <v>224.87087356009175</v>
       </c>
       <c r="F105" s="4">
         <v>4.7213636363636367</v>
@@ -4244,7 +4244,7 @@
         <v>4.2</v>
       </c>
       <c r="E106" s="6">
-        <v>177.8</v>
+        <v>224.99317566341949</v>
       </c>
       <c r="F106" s="4">
         <v>4.6761904761904765</v>
@@ -4271,7 +4271,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E107" s="6">
-        <v>178.1</v>
+        <v>225.06639194632436</v>
       </c>
       <c r="F107" s="4">
         <v>4.8609999999999998</v>
@@ -4298,7 +4298,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E108" s="6">
-        <v>178.4</v>
+        <v>225.13948500401045</v>
       </c>
       <c r="F108" s="4">
         <v>5.0705</v>
@@ -4325,7 +4325,7 @@
         <v>4</v>
       </c>
       <c r="E109" s="6">
-        <v>178.7</v>
+        <v>225.2124552505644</v>
       </c>
       <c r="F109" s="4">
         <v>5.1963636363636363</v>
@@ -4352,7 +4352,7 @@
         <v>4</v>
       </c>
       <c r="E110" s="6">
-        <v>179.3</v>
+        <v>225.35802895621831</v>
       </c>
       <c r="F110" s="4">
         <v>5.3185000000000002</v>
@@ -4379,7 +4379,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E111" s="6">
-        <v>179.4</v>
+        <v>225.38224387080734</v>
       </c>
       <c r="F111" s="4">
         <v>5.548</v>
@@ -4406,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="E112" s="6">
-        <v>180</v>
+        <v>225.52725051033059</v>
       </c>
       <c r="F112" s="4">
         <v>5.6947826086956521</v>
@@ -4433,7 +4433,7 @@
         <v>3.8</v>
       </c>
       <c r="E113" s="6">
-        <v>180.3</v>
+        <v>225.59957267224019</v>
       </c>
       <c r="F113" s="4">
         <v>5.6584210526315788</v>
@@ -4460,7 +4460,7 @@
         <v>4</v>
       </c>
       <c r="E114" s="6">
-        <v>180.7</v>
+        <v>225.6958152560932</v>
       </c>
       <c r="F114" s="4">
         <v>5.790909090909091</v>
@@ -4487,7 +4487,7 @@
         <v>4</v>
       </c>
       <c r="E115" s="6">
-        <v>181.1</v>
+        <v>225.79184503140587</v>
       </c>
       <c r="F115" s="4">
         <v>5.6863636363636365</v>
@@ -4514,7 +4514,7 @@
         <v>4</v>
       </c>
       <c r="E116" s="6">
-        <v>181.5</v>
+        <v>225.88766293721312</v>
       </c>
       <c r="F116" s="4">
         <v>5.9550000000000001</v>
@@ -4541,7 +4541,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E117" s="6">
-        <v>181.9</v>
+        <v>225.98326990634834</v>
       </c>
       <c r="F117" s="4">
         <v>6.0943478260869561</v>
@@ -4568,7 +4568,7 @@
         <v>3.9</v>
       </c>
       <c r="E118" s="6">
-        <v>182.3</v>
+        <v>226.07866686549761</v>
       </c>
       <c r="F118" s="4">
         <v>5.9974999999999996</v>
@@ -4595,7 +4595,7 @@
         <v>3.9</v>
       </c>
       <c r="E119" s="6">
-        <v>182.6</v>
+        <v>226.150077319828</v>
       </c>
       <c r="F119" s="4">
         <v>6.1066666666666665</v>
@@ -4622,7 +4622,7 @@
         <v>3.9</v>
       </c>
       <c r="E120" s="6">
-        <v>183.1</v>
+        <v>226.26883443016962</v>
       </c>
       <c r="F120" s="4">
         <v>6.171904761904762</v>
@@ -4649,7 +4649,7 @@
         <v>3.9</v>
       </c>
       <c r="E121" s="6">
-        <v>183.3</v>
+        <v>226.31624649622165</v>
       </c>
       <c r="F121" s="4">
         <v>5.7690000000000001</v>
@@ -4676,7 +4676,7 @@
         <v>4.2</v>
       </c>
       <c r="E122" s="6">
-        <v>183.9</v>
+        <v>226.45817292380775</v>
       </c>
       <c r="F122" s="4">
         <v>5.1457142857142859</v>
@@ -4703,7 +4703,7 @@
         <v>4.2</v>
       </c>
       <c r="E123" s="6">
-        <v>184.4</v>
+        <v>226.57609167176105</v>
       </c>
       <c r="F123" s="4">
         <v>4.8815789473684212</v>
@@ -4730,7 +4730,7 @@
         <v>4.3</v>
       </c>
       <c r="E124" s="6">
-        <v>184.7</v>
+        <v>226.64668954402413</v>
       </c>
       <c r="F124" s="4">
         <v>4.4245454545454548</v>
@@ -4757,7 +4757,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E125" s="6">
-        <v>185.1</v>
+        <v>226.74064187529041</v>
       </c>
       <c r="F125" s="4">
         <v>3.8725000000000001</v>
@@ -4784,7 +4784,7 @@
         <v>4.3</v>
       </c>
       <c r="E126" s="6">
-        <v>185.3</v>
+        <v>226.78754193188973</v>
       </c>
       <c r="F126" s="4">
         <v>3.6204545454545456</v>
@@ -4811,7 +4811,7 @@
         <v>4.5</v>
       </c>
       <c r="E127" s="6">
-        <v>186</v>
+        <v>226.95129442179166</v>
       </c>
       <c r="F127" s="4">
         <v>3.485238095238095</v>
@@ -4838,7 +4838,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E128" s="6">
-        <v>186.4</v>
+        <v>227.04459080179626</v>
       </c>
       <c r="F128" s="4">
         <v>3.5133333333333332</v>
@@ -4865,7 +4865,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E129" s="6">
-        <v>186.7</v>
+        <v>227.11443179490783</v>
       </c>
       <c r="F129" s="4">
         <v>3.3617391304347826</v>
@@ -4892,7 +4892,7 @@
         <v>5</v>
       </c>
       <c r="E130" s="6">
-        <v>187.1</v>
+        <v>227.207378750001</v>
       </c>
       <c r="F130" s="4">
         <v>2.6364705882352939</v>
@@ -4919,7 +4919,7 @@
         <v>5.3</v>
       </c>
       <c r="E131" s="6">
-        <v>187.4</v>
+        <v>227.27695865517595</v>
       </c>
       <c r="F131" s="4">
         <v>2.1572727272727272</v>
@@ -4946,7 +4946,7 @@
         <v>5.5</v>
       </c>
       <c r="E132" s="6">
-        <v>188.1</v>
+        <v>227.43887955503789</v>
       </c>
       <c r="F132" s="4">
         <v>1.871</v>
@@ -4973,7 +4973,7 @@
         <v>5.7</v>
       </c>
       <c r="E133" s="6">
-        <v>188.4</v>
+        <v>227.50808984568587</v>
       </c>
       <c r="F133" s="4">
         <v>1.69</v>
@@ -5000,7 +5000,7 @@
         <v>5.7</v>
       </c>
       <c r="E134" s="6">
-        <v>188.7</v>
+        <v>227.57719001649312</v>
       </c>
       <c r="F134" s="4">
         <v>1.6533333333333333</v>
@@ -5027,7 +5027,7 @@
         <v>5.7</v>
       </c>
       <c r="E135" s="6">
-        <v>189.1</v>
+        <v>227.66915288450397</v>
       </c>
       <c r="F135" s="4">
         <v>1.7247368421052631</v>
@@ -5054,7 +5054,7 @@
         <v>5.7</v>
       </c>
       <c r="E136" s="6">
-        <v>189.2</v>
+        <v>227.6921132065774</v>
       </c>
       <c r="F136" s="4">
         <v>1.7875000000000001</v>
@@ -5081,7 +5081,7 @@
         <v>5.9</v>
       </c>
       <c r="E137" s="6">
-        <v>189.7</v>
+        <v>227.80673308886628</v>
       </c>
       <c r="F137" s="4">
         <v>1.7136363636363636</v>
@@ -5108,7 +5108,7 @@
         <v>5.8</v>
       </c>
       <c r="E138" s="6">
-        <v>190</v>
+        <v>227.87536009528287</v>
       </c>
       <c r="F138" s="4">
         <v>1.7272727272727273</v>
@@ -5135,7 +5135,7 @@
         <v>5.8</v>
       </c>
       <c r="E139" s="6">
-        <v>190.2</v>
+        <v>227.92105126013951</v>
       </c>
       <c r="F139" s="4">
         <v>1.6995</v>
@@ -5162,7 +5162,7 @@
         <v>5.8</v>
       </c>
       <c r="E140" s="6">
-        <v>190.5</v>
+        <v>227.98949800116381</v>
       </c>
       <c r="F140" s="4">
         <v>1.6831818181818181</v>
@@ -5189,7 +5189,7 @@
         <v>5.7</v>
       </c>
       <c r="E141" s="6">
-        <v>191.1</v>
+        <v>228.1260687055013</v>
       </c>
       <c r="F141" s="4">
         <v>1.615909090909091</v>
@@ -5216,7 +5216,7 @@
         <v>5.7</v>
       </c>
       <c r="E142" s="6">
-        <v>191.3</v>
+        <v>228.17149700272958</v>
       </c>
       <c r="F142" s="4">
         <v>1.629</v>
@@ -5243,7 +5243,7 @@
         <v>5.7</v>
       </c>
       <c r="E143" s="6">
-        <v>191.5</v>
+        <v>228.21687783046417</v>
       </c>
       <c r="F143" s="4">
         <v>1.5804545454545456</v>
@@ -5270,7 +5270,7 @@
         <v>5.9</v>
       </c>
       <c r="E144" s="6">
-        <v>191.9</v>
+        <v>228.30749747354716</v>
       </c>
       <c r="F144" s="4">
         <v>1.2347368421052631</v>
@@ -5297,7 +5297,7 @@
         <v>6</v>
       </c>
       <c r="E145" s="6">
-        <v>192.1</v>
+        <v>228.35273648616936</v>
       </c>
       <c r="F145" s="4">
         <v>1.190952380952381</v>
@@ -5324,7 +5324,7 @@
         <v>5.8</v>
       </c>
       <c r="E146" s="6">
-        <v>192.4</v>
+        <v>228.4205067701794</v>
       </c>
       <c r="F146" s="4">
         <v>1.1690476190476189</v>
@@ -5351,7 +5351,7 @@
         <v>5.9</v>
       </c>
       <c r="E147" s="6">
-        <v>192.5</v>
+        <v>228.44307338445194</v>
       </c>
       <c r="F147" s="4">
         <v>1.1652631578947368</v>
@@ -5378,7 +5378,7 @@
         <v>5.9</v>
       </c>
       <c r="E148" s="6">
-        <v>192.5</v>
+        <v>228.44307338445194</v>
       </c>
       <c r="F148" s="4">
         <v>1.1309523809523809</v>
@@ -5405,7 +5405,7 @@
         <v>6</v>
       </c>
       <c r="E149" s="6">
-        <v>192.5</v>
+        <v>228.44307338445194</v>
       </c>
       <c r="F149" s="4">
         <v>1.1323809523809525</v>
@@ -5432,7 +5432,7 @@
         <v>6.1</v>
       </c>
       <c r="E150" s="6">
-        <v>192.9</v>
+        <v>228.53322276438846</v>
       </c>
       <c r="F150" s="4">
         <v>1.0680952380952382</v>
@@ -5459,7 +5459,7 @@
         <v>6.3</v>
       </c>
       <c r="E151" s="6">
-        <v>193</v>
+        <v>228.55573090077738</v>
       </c>
       <c r="F151" s="4">
         <v>0.91714285714285715</v>
@@ -5486,7 +5486,7 @@
         <v>6.2</v>
       </c>
       <c r="E152" s="6">
-        <v>193.4</v>
+        <v>228.64564697469828</v>
       </c>
       <c r="F152" s="4">
         <v>0.90045454545454551</v>
@@ -5513,7 +5513,7 @@
         <v>6.1</v>
       </c>
       <c r="E153" s="6">
-        <v>193.6</v>
+        <v>228.69053529723749</v>
       </c>
       <c r="F153" s="4">
         <v>0.94904761904761903</v>
@@ -5540,7 +5540,7 @@
         <v>6.1</v>
       </c>
       <c r="E154" s="6">
-        <v>193.7</v>
+        <v>228.71296207191111</v>
       </c>
       <c r="F154" s="4">
         <v>0.93666666666666665</v>
@@ -5567,7 +5567,7 @@
         <v>6</v>
       </c>
       <c r="E155" s="6">
-        <v>194</v>
+        <v>228.7801729930226</v>
       </c>
       <c r="F155" s="4">
         <v>0.92181818181818187</v>
@@ -5594,7 +5594,7 @@
         <v>5.8</v>
       </c>
       <c r="E156" s="6">
-        <v>194</v>
+        <v>228.7801729930226</v>
       </c>
       <c r="F156" s="4">
         <v>0.93222222222222217</v>
@@ -5621,7 +5621,7 @@
         <v>5.7</v>
       </c>
       <c r="E157" s="6">
-        <v>194.2</v>
+        <v>228.82492255719859</v>
       </c>
       <c r="F157" s="4">
         <v>0.89590909090909088</v>
@@ -5648,7 +5648,7 @@
         <v>5.7</v>
       </c>
       <c r="E158" s="6">
-        <v>194.6</v>
+        <v>228.91428359323331</v>
       </c>
       <c r="F158" s="4">
         <v>0.88300000000000001</v>
@@ -5675,7 +5675,7 @@
         <v>5.6</v>
       </c>
       <c r="E159" s="6">
-        <v>194.9</v>
+        <v>228.98118391176214</v>
       </c>
       <c r="F159" s="4">
         <v>0.9257894736842105</v>
@@ -5702,7 +5702,7 @@
         <v>5.8</v>
       </c>
       <c r="E160" s="6">
-        <v>195.5</v>
+        <v>229.11467617318854</v>
       </c>
       <c r="F160" s="4">
         <v>0.93695652173913047</v>
@@ -5729,7 +5729,7 @@
         <v>5.6</v>
       </c>
       <c r="E161" s="6">
-        <v>195.9</v>
+        <v>229.20344359947364</v>
       </c>
       <c r="F161" s="4">
         <v>0.94380952380952376</v>
@@ -5756,7 +5756,7 @@
         <v>5.6</v>
       </c>
       <c r="E162" s="6">
-        <v>196.2</v>
+        <v>229.26990030439299</v>
       </c>
       <c r="F162" s="4">
         <v>1.0235000000000001</v>
@@ -5783,7 +5783,7 @@
         <v>5.6</v>
       </c>
       <c r="E163" s="6">
-        <v>196.6</v>
+        <v>229.35835134961167</v>
       </c>
       <c r="F163" s="4">
         <v>1.2666666666666666</v>
@@ -5810,7 +5810,7 @@
         <v>5.5</v>
       </c>
       <c r="E164" s="6">
-        <v>196.8</v>
+        <v>229.40250940953226</v>
       </c>
       <c r="F164" s="4">
         <v>1.3333333333333333</v>
@@ -5837,7 +5837,7 @@
         <v>5.4</v>
       </c>
       <c r="E165" s="6">
-        <v>196.9</v>
+        <v>229.42457161381182</v>
       </c>
       <c r="F165" s="4">
         <v>1.479090909090909</v>
@@ -5864,7 +5864,7 @@
         <v>5.4</v>
       </c>
       <c r="E166" s="6">
-        <v>197.5</v>
+        <v>229.55670999624789</v>
       </c>
       <c r="F166" s="4">
         <v>1.6528571428571428</v>
@@ -5891,7 +5891,7 @@
         <v>5.5</v>
       </c>
       <c r="E167" s="6">
-        <v>197.9</v>
+        <v>229.64457942063964</v>
       </c>
       <c r="F167" s="4">
         <v>1.7609999999999999</v>
@@ -5918,7 +5918,7 @@
         <v>5.4</v>
       </c>
       <c r="E168" s="6">
-        <v>198.3</v>
+        <v>229.73227142053028</v>
       </c>
       <c r="F168" s="4">
         <v>2.069</v>
@@ -5945,7 +5945,7 @@
         <v>5.4</v>
       </c>
       <c r="E169" s="6">
-        <v>198.6</v>
+        <v>229.79792441593622</v>
       </c>
       <c r="F169" s="4">
         <v>2.1872727272727275</v>
@@ -5972,7 +5972,7 @@
         <v>5.3</v>
       </c>
       <c r="E170" s="6">
-        <v>199</v>
+        <v>229.88530764097069</v>
       </c>
       <c r="F170" s="4">
         <v>2.3334999999999999</v>
@@ -5999,7 +5999,7 @@
         <v>5.4</v>
       </c>
       <c r="E171" s="6">
-        <v>199.4</v>
+        <v>229.97251539756371</v>
       </c>
       <c r="F171" s="4">
         <v>2.5389473684210526</v>
@@ -6026,7 +6026,7 @@
         <v>5.2</v>
       </c>
       <c r="E172" s="6">
-        <v>200.1</v>
+        <v>230.12470886362112</v>
       </c>
       <c r="F172" s="4">
         <v>2.7386363636363638</v>
@@ -6053,7 +6053,7 @@
         <v>5.2</v>
       </c>
       <c r="E173" s="6">
-        <v>200.2</v>
+        <v>230.14640731432996</v>
       </c>
       <c r="F173" s="4">
         <v>2.7809523809523808</v>
@@ -6080,7 +6080,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E174" s="6">
-        <v>200.5</v>
+        <v>230.21143769562008</v>
       </c>
       <c r="F174" s="4">
         <v>2.8414285714285712</v>
@@ -6107,7 +6107,7 @@
         <v>5</v>
       </c>
       <c r="E175" s="6">
-        <v>200.6</v>
+        <v>230.23309286843991</v>
       </c>
       <c r="F175" s="4">
         <v>2.9727272727272727</v>
@@ -6134,7 +6134,7 @@
         <v>5</v>
       </c>
       <c r="E176" s="6">
-        <v>200.9</v>
+        <v>230.29799367482494</v>
       </c>
       <c r="F176" s="4">
         <v>3.2155</v>
@@ -6161,7 +6161,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E177" s="6">
-        <v>201.1</v>
+        <v>230.34120705967419</v>
       </c>
       <c r="F177" s="4">
         <v>3.4408695652173913</v>
@@ -6188,7 +6188,7 @@
         <v>5</v>
       </c>
       <c r="E178" s="6">
-        <v>201.3</v>
+        <v>230.38437748886545</v>
       </c>
       <c r="F178" s="4">
         <v>3.4195238095238096</v>
@@ -6215,7 +6215,7 @@
         <v>5</v>
       </c>
       <c r="E179" s="6">
-        <v>202</v>
+        <v>230.53513694466238</v>
       </c>
       <c r="F179" s="4">
         <v>3.706</v>
@@ -6242,7 +6242,7 @@
         <v>5</v>
       </c>
       <c r="E180" s="6">
-        <v>202.5</v>
+        <v>230.64250275506873</v>
       </c>
       <c r="F180" s="4">
         <v>3.8835000000000002</v>
@@ -6269,7 +6269,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E181" s="6">
-        <v>202.8</v>
+        <v>230.70679506612984</v>
       </c>
       <c r="F181" s="4">
         <v>3.8861904761904764</v>
@@ -6296,7 +6296,7 @@
         <v>4.7</v>
       </c>
       <c r="E182" s="6">
-        <v>203.2</v>
+        <v>230.79237036118818</v>
       </c>
       <c r="F182" s="4">
         <v>4.2359999999999998</v>
@@ -6323,7 +6323,7 @@
         <v>4.8</v>
       </c>
       <c r="E183" s="6">
-        <v>203.6</v>
+        <v>230.87777736647212</v>
       </c>
       <c r="F183" s="4">
         <v>4.4331578947368424</v>
@@ -6350,7 +6350,7 @@
         <v>4.7</v>
       </c>
       <c r="E184" s="6">
-        <v>204.3</v>
+        <v>231.02683666324478</v>
       </c>
       <c r="F184" s="4">
         <v>4.5121739130434779</v>
@@ -6377,7 +6377,7 @@
         <v>4.7</v>
       </c>
       <c r="E185" s="6">
-        <v>204.8</v>
+        <v>231.13299523037932</v>
       </c>
       <c r="F185" s="4">
         <v>4.6036842105263158</v>
@@ -6404,7 +6404,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E186" s="6">
-        <v>205.4</v>
+        <v>231.26004392612595</v>
       </c>
       <c r="F186" s="4">
         <v>4.7154545454545458</v>
@@ -6431,7 +6431,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E187" s="6">
-        <v>205.9</v>
+        <v>231.36563466180314</v>
       </c>
       <c r="F187" s="4">
         <v>4.791363636363636</v>
@@ -6458,7 +6458,7 @@
         <v>4.7</v>
       </c>
       <c r="E188" s="6">
-        <v>206.3</v>
+        <v>231.44992279731517</v>
       </c>
       <c r="F188" s="4">
         <v>4.9465000000000003</v>
@@ -6485,7 +6485,7 @@
         <v>4.7</v>
       </c>
       <c r="E189" s="6">
-        <v>206.8</v>
+        <v>231.55505344219048</v>
       </c>
       <c r="F189" s="4">
         <v>4.9604347826086954</v>
@@ -6512,7 +6512,7 @@
         <v>4.5</v>
       </c>
       <c r="E190" s="6">
-        <v>207.2</v>
+        <v>231.63897510731951</v>
       </c>
       <c r="F190" s="4">
         <v>4.8055000000000003</v>
@@ -6539,7 +6539,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E191" s="6">
-        <v>207.6</v>
+        <v>231.72273491764201</v>
       </c>
       <c r="F191" s="4">
         <v>4.9171428571428573</v>
@@ -6566,7 +6566,7 @@
         <v>4.5</v>
       </c>
       <c r="E192" s="6">
-        <v>207.8</v>
+        <v>231.76455432211586</v>
       </c>
       <c r="F192" s="4">
         <v>4.9433333333333334</v>
@@ -6593,7 +6593,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E193" s="6">
-        <v>208.1</v>
+        <v>231.8272080211627</v>
       </c>
       <c r="F193" s="4">
         <v>4.8475000000000001</v>
@@ -6620,7 +6620,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E194" s="6">
-        <v>208.6</v>
+        <v>231.93143040905122</v>
       </c>
       <c r="F194" s="4">
         <v>4.9752380952380948</v>
@@ -6647,7 +6647,7 @@
         <v>4.5</v>
       </c>
       <c r="E195" s="6">
-        <v>209.13499999999999</v>
+        <v>232.04267206936368</v>
       </c>
       <c r="F195" s="4">
         <v>5.0268421052631576</v>
@@ -6674,7 +6674,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E196" s="6">
-        <v>209.41800000000001</v>
+        <v>232.10140076422809</v>
       </c>
       <c r="F196" s="4">
         <v>4.9390909090909094</v>
@@ -6701,7 +6701,7 @@
         <v>4.5</v>
       </c>
       <c r="E197" s="6">
-        <v>209.74700000000001</v>
+        <v>232.1695757854668</v>
       </c>
       <c r="F197" s="4">
         <v>4.8690476190476186</v>
@@ -6728,7 +6728,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E198" s="6">
-        <v>210.05799999999999</v>
+        <v>232.23392261724848</v>
       </c>
       <c r="F198" s="4">
         <v>4.7327272727272724</v>
@@ -6755,7 +6755,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E199" s="6">
-        <v>210.392</v>
+        <v>232.3029222069585</v>
       </c>
       <c r="F199" s="4">
         <v>4.6109523809523809</v>
@@ -6782,7 +6782,7 @@
         <v>4.7</v>
       </c>
       <c r="E200" s="6">
-        <v>210.773</v>
+        <v>232.38149770242572</v>
       </c>
       <c r="F200" s="4">
         <v>4.8214285714285712</v>
@@ -6809,7 +6809,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E201" s="6">
-        <v>211.119</v>
+        <v>232.45273201093482</v>
       </c>
       <c r="F201" s="4">
         <v>4.2017391304347829</v>
@@ -6836,7 +6836,7 @@
         <v>4.7</v>
       </c>
       <c r="E202" s="6">
-        <v>211.554</v>
+        <v>232.5421241255612</v>
       </c>
       <c r="F202" s="4">
         <v>3.8921052631578945</v>
@@ -6863,7 +6863,7 @@
         <v>4.7</v>
       </c>
       <c r="E203" s="6">
-        <v>212.077</v>
+        <v>232.64935713232035</v>
       </c>
       <c r="F203" s="4">
         <v>3.8995454545454544</v>
@@ -6890,7 +6890,7 @@
         <v>4.7</v>
       </c>
       <c r="E204" s="6">
-        <v>212.66</v>
+        <v>232.76858095410242</v>
       </c>
       <c r="F204" s="4">
         <v>3.2730000000000001</v>
@@ -6917,7 +6917,7 @@
         <v>5</v>
       </c>
       <c r="E205" s="6">
-        <v>213.16800000000001</v>
+        <v>232.87220105492631</v>
       </c>
       <c r="F205" s="4">
         <v>2.9954999999999998</v>
@@ -6944,7 +6944,7 @@
         <v>5</v>
       </c>
       <c r="E206" s="6">
-        <v>213.77099999999999</v>
+        <v>232.99487888324455</v>
       </c>
       <c r="F206" s="4">
         <v>2.7533333333333334</v>
@@ -6971,7 +6971,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E207" s="6">
-        <v>213.93899999999999</v>
+        <v>233.0289961480791</v>
       </c>
       <c r="F207" s="4">
         <v>2.1244999999999998</v>
@@ -6998,7 +6998,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E208" s="6">
-        <v>214.42</v>
+        <v>233.12652916762261</v>
       </c>
       <c r="F208" s="4">
         <v>1.2625</v>
@@ -7025,7 +7025,7 @@
         <v>5</v>
       </c>
       <c r="E209" s="6">
-        <v>214.56</v>
+        <v>233.15487605075239</v>
       </c>
       <c r="F209" s="4">
         <v>1.2936363636363637</v>
@@ -7052,7 +7052,7 @@
         <v>5.4</v>
       </c>
       <c r="E210" s="6">
-        <v>214.93600000000001</v>
+        <v>233.23091623129523</v>
       </c>
       <c r="F210" s="4">
         <v>1.7338095238095237</v>
@@ -7079,7 +7079,7 @@
         <v>5.6</v>
       </c>
       <c r="E211" s="6">
-        <v>215.42400000000001</v>
+        <v>233.32940856236922</v>
       </c>
       <c r="F211" s="4">
         <v>1.8561904761904762</v>
@@ -7106,7 +7106,7 @@
         <v>5.8</v>
       </c>
       <c r="E212" s="6">
-        <v>215.965</v>
+        <v>233.43833736578478</v>
       </c>
       <c r="F212" s="4">
         <v>1.625909090909091</v>
@@ -7133,7 +7133,7 @@
         <v>6.1</v>
       </c>
       <c r="E213" s="6">
-        <v>216.393</v>
+        <v>233.52432078645523</v>
       </c>
       <c r="F213" s="4">
         <v>1.7219047619047618</v>
@@ -7160,7 +7160,7 @@
         <v>6.1</v>
       </c>
       <c r="E214" s="6">
-        <v>216.71299999999999</v>
+        <v>233.58849641990184</v>
       </c>
       <c r="F214" s="4">
         <v>1.1342857142857143</v>
@@ -7187,7 +7187,7 @@
         <v>6.5</v>
       </c>
       <c r="E215" s="6">
-        <v>216.78800000000001</v>
+        <v>233.60352387610965</v>
       </c>
       <c r="F215" s="4">
         <v>0.67454545454545456</v>
@@ -7214,7 +7214,7 @@
         <v>6.8</v>
       </c>
       <c r="E216" s="6">
-        <v>216.947</v>
+        <v>233.63536489687849</v>
       </c>
       <c r="F216" s="4">
         <v>0.19111111111111112</v>
@@ -7241,7 +7241,7 @@
         <v>7.3</v>
       </c>
       <c r="E217" s="6">
-        <v>216.92500000000001</v>
+        <v>233.6309606123844</v>
       </c>
       <c r="F217" s="4">
         <v>3.4545454545454546E-2</v>
@@ -7268,7 +7268,7 @@
         <v>7.8</v>
       </c>
       <c r="E218" s="6">
-        <v>217.346</v>
+        <v>233.71516519162606</v>
       </c>
       <c r="F218" s="4">
         <v>0.13</v>
@@ -7295,7 +7295,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="E219" s="6">
-        <v>217.792</v>
+        <v>233.80419230796969</v>
       </c>
       <c r="F219" s="4">
         <v>0.29578947368421055</v>
@@ -7322,7 +7322,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E220" s="6">
-        <v>218.25299999999999</v>
+        <v>233.89602220201789</v>
       </c>
       <c r="F220" s="4">
         <v>0.21363636363636362</v>
@@ -7349,7 +7349,7 @@
         <v>9</v>
       </c>
       <c r="E221" s="6">
-        <v>218.70599999999999</v>
+        <v>233.98606976748005</v>
       </c>
       <c r="F221" s="4">
         <v>0.15809523809523809</v>
@@ -7376,7 +7376,7 @@
         <v>9.4</v>
       </c>
       <c r="E222" s="6">
-        <v>218.904</v>
+        <v>234.02536974384475</v>
       </c>
       <c r="F222" s="4">
         <v>0.17599999999999999</v>
@@ -7403,7 +7403,7 @@
         <v>9.5</v>
       </c>
       <c r="E223" s="6">
-        <v>219.11199999999999</v>
+        <v>234.06661630060336</v>
       </c>
       <c r="F223" s="4">
         <v>0.17681818181818182</v>
@@ -7430,7 +7430,7 @@
         <v>9.5</v>
       </c>
       <c r="E224" s="6">
-        <v>219.26300000000001</v>
+        <v>234.09653519167199</v>
       </c>
       <c r="F224" s="4">
         <v>0.18363636363636363</v>
@@ -7457,7 +7457,7 @@
         <v>9.6</v>
       </c>
       <c r="E225" s="6">
-        <v>219.49600000000001</v>
+        <v>234.1426610255788</v>
       </c>
       <c r="F225" s="4">
         <v>0.17142857142857143</v>
@@ -7484,7 +7484,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="E226" s="6">
-        <v>219.92</v>
+        <v>234.2264726835412</v>
       </c>
       <c r="F226" s="4">
         <v>0.12333333333333334</v>
@@ -7511,7 +7511,7 @@
         <v>10</v>
       </c>
       <c r="E227" s="6">
-        <v>220.501</v>
+        <v>234.34105633888782</v>
       </c>
       <c r="F227" s="4">
         <v>7.4285714285714288E-2</v>
@@ -7538,7 +7538,7 @@
         <v>9.9</v>
       </c>
       <c r="E228" s="6">
-        <v>220.666</v>
+        <v>234.37354226501347</v>
       </c>
       <c r="F228" s="4">
         <v>5.2105263157894738E-2</v>
@@ -7565,7 +7565,7 @@
         <v>9.9</v>
       </c>
       <c r="E229" s="6">
-        <v>220.881</v>
+        <v>234.41583598277788</v>
       </c>
       <c r="F229" s="4">
         <v>5.4545454545454543E-2</v>
@@ -7592,7 +7592,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="E230" s="6">
-        <v>220.63300000000001</v>
+        <v>234.36704702349712</v>
       </c>
       <c r="F230" s="4">
         <v>6.1578947368421053E-2</v>
@@ -7619,7 +7619,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="E231" s="6">
-        <v>220.73099999999999</v>
+        <v>234.38633308213625</v>
       </c>
       <c r="F231" s="4">
         <v>0.10894736842105263</v>
@@ -7646,7 +7646,7 @@
         <v>9.9</v>
       </c>
       <c r="E232" s="6">
-        <v>220.78299999999999</v>
+        <v>234.39656302418265</v>
       </c>
       <c r="F232" s="4">
         <v>0.15043478260869564</v>
@@ -7673,7 +7673,7 @@
         <v>9.9</v>
       </c>
       <c r="E233" s="6">
-        <v>220.822</v>
+        <v>234.4042338996656</v>
       </c>
       <c r="F233" s="4">
         <v>0.16227272727272726</v>
@@ -7700,7 +7700,7 @@
         <v>9.6</v>
       </c>
       <c r="E234" s="6">
-        <v>220.96199999999999</v>
+        <v>234.43175921950595</v>
       </c>
       <c r="F234" s="4">
         <v>0.16</v>
@@ -7727,7 +7727,7 @@
         <v>9.4</v>
       </c>
       <c r="E235" s="6">
-        <v>221.19399999999999</v>
+        <v>234.47733423332375</v>
       </c>
       <c r="F235" s="4">
         <v>0.12363636363636364</v>
@@ -7754,7 +7754,7 @@
         <v>9.4</v>
       </c>
       <c r="E236" s="6">
-        <v>221.363</v>
+        <v>234.51050319054701</v>
       </c>
       <c r="F236" s="4">
         <v>0.15761904761904763</v>
@@ -7781,7 +7781,7 @@
         <v>9.5</v>
       </c>
       <c r="E237" s="6">
-        <v>221.50899999999999</v>
+        <v>234.53913764775129</v>
       </c>
       <c r="F237" s="4">
         <v>0.155</v>
@@ -7808,7 +7808,7 @@
         <v>9.5</v>
       </c>
       <c r="E238" s="6">
-        <v>221.71100000000001</v>
+        <v>234.5787240795091</v>
       </c>
       <c r="F238" s="4">
         <v>0.1519047619047619</v>
@@ -7835,7 +7835,7 @@
         <v>9.4</v>
       </c>
       <c r="E239" s="6">
-        <v>221.83</v>
+        <v>234.60202792045575</v>
       </c>
       <c r="F239" s="4">
         <v>0.13450000000000001</v>
@@ -7862,7 +7862,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="E240" s="6">
-        <v>222.149</v>
+        <v>234.6644362611959</v>
       </c>
       <c r="F240" s="4">
         <v>0.14299999999999999</v>
@@ -7889,7 +7889,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="E241" s="6">
-        <v>222.34299999999999</v>
+        <v>234.70234611551905</v>
       </c>
       <c r="F241" s="4">
         <v>0.1409090909090909</v>
@@ -7916,7 +7916,7 @@
         <v>9.1</v>
       </c>
       <c r="E242" s="6">
-        <v>222.803</v>
+        <v>234.79210342336216</v>
       </c>
       <c r="F242" s="4">
         <v>0.152</v>
@@ -7943,7 +7943,7 @@
         <v>9</v>
       </c>
       <c r="E243" s="6">
-        <v>223.21299999999999</v>
+        <v>234.87194844584357</v>
       </c>
       <c r="F243" s="4">
         <v>0.13210526315789473</v>
@@ -7970,7 +7970,7 @@
         <v>9</v>
       </c>
       <c r="E244" s="6">
-        <v>223.45400000000001</v>
+        <v>234.91881332741991</v>
       </c>
       <c r="F244" s="4">
         <v>0.10043478260869565</v>
@@ -7997,7 +7997,7 @@
         <v>9.1</v>
       </c>
       <c r="E245" s="6">
-        <v>223.727</v>
+        <v>234.97183991320463</v>
       </c>
       <c r="F245" s="4">
         <v>5.8500000000000003E-2</v>
@@ -8024,7 +8024,7 @@
         <v>9</v>
       </c>
       <c r="E246" s="6">
-        <v>224.17500000000001</v>
+        <v>235.05871784309807</v>
       </c>
       <c r="F246" s="4">
         <v>4.0952380952380955E-2</v>
@@ -8051,7 +8051,7 @@
         <v>9.1</v>
       </c>
       <c r="E247" s="6">
-        <v>224.697</v>
+        <v>235.15972740562304</v>
       </c>
       <c r="F247" s="4">
         <v>3.727272727272727E-2</v>
@@ -8078,7 +8078,7 @@
         <v>9</v>
       </c>
       <c r="E248" s="6">
-        <v>225.21799999999999</v>
+        <v>235.26030974949239</v>
       </c>
       <c r="F248" s="4">
         <v>3.7499999999999999E-2</v>
@@ -8105,7 +8105,7 @@
         <v>9</v>
       </c>
       <c r="E249" s="6">
-        <v>225.86199999999999</v>
+        <v>235.38431694838047</v>
       </c>
       <c r="F249" s="4">
         <v>2.4347826086956521E-2</v>
@@ -8132,7 +8132,7 @@
         <v>9</v>
       </c>
       <c r="E250" s="6">
-        <v>226.11799999999999</v>
+        <v>235.43351354967089</v>
       </c>
       <c r="F250" s="4">
         <v>1.380952380952381E-2</v>
@@ -8159,7 +8159,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="E251" s="6">
-        <v>226.506</v>
+        <v>235.50797106860628</v>
       </c>
       <c r="F251" s="4">
         <v>1.9E-2</v>
@@ -8186,7 +8186,7 @@
         <v>8.6</v>
       </c>
       <c r="E252" s="6">
-        <v>226.899</v>
+        <v>235.58325818459807</v>
       </c>
       <c r="F252" s="4">
         <v>1.4E-2</v>
@@ -8213,7 +8213,7 @@
         <v>8.5</v>
       </c>
       <c r="E253" s="6">
-        <v>227.405</v>
+        <v>235.68000093778244</v>
       </c>
       <c r="F253" s="4">
         <v>1.1428571428571429E-2</v>
@@ -8240,7 +8240,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="E254" s="6">
-        <v>227.87700000000001</v>
+        <v>235.7700493336767</v>
       </c>
       <c r="F254" s="4">
         <v>3.4500000000000003E-2</v>
@@ -8267,7 +8267,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="E255" s="6">
-        <v>228.03399999999999</v>
+        <v>235.79996053843115</v>
       </c>
       <c r="F255" s="4">
         <v>9.1999999999999998E-2</v>
@@ -8294,7 +8294,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E256" s="6">
-        <v>228.47800000000001</v>
+        <v>235.88443884820859</v>
       </c>
       <c r="F256" s="4">
         <v>8.4090909090909091E-2</v>
@@ -8321,7 +8321,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E257" s="6">
-        <v>228.905</v>
+        <v>235.96552791258028</v>
       </c>
       <c r="F257" s="4">
         <v>8.3809523809523806E-2</v>
@@ -8348,7 +8348,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E258" s="6">
-        <v>229.22399999999999</v>
+        <v>236.02600867765625</v>
       </c>
       <c r="F258" s="4">
         <v>8.9545454545454539E-2</v>
@@ -8375,7 +8375,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E259" s="6">
-        <v>229.62299999999999</v>
+        <v>236.10153866562862</v>
       </c>
       <c r="F259" s="4">
         <v>9.1428571428571428E-2</v>
@@ -8402,7 +8402,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E260" s="6">
-        <v>229.97</v>
+        <v>236.16711852165596</v>
       </c>
       <c r="F260" s="4">
         <v>9.7142857142857142E-2</v>
@@ -8429,7 +8429,7 @@
         <v>8.1</v>
       </c>
       <c r="E261" s="6">
-        <v>230.233</v>
+        <v>236.21675725116239</v>
       </c>
       <c r="F261" s="4">
         <v>0.10260869565217391</v>
@@ -8456,7 +8456,7 @@
         <v>7.8</v>
       </c>
       <c r="E262" s="6">
-        <v>230.65899999999999</v>
+        <v>236.29704048540233</v>
       </c>
       <c r="F262" s="4">
         <v>0.10526315789473684</v>
@@ -8483,7 +8483,7 @@
         <v>7.8</v>
       </c>
       <c r="E263" s="6">
-        <v>231.024</v>
+        <v>236.36570990529458</v>
       </c>
       <c r="F263" s="4">
         <v>0.10476190476190476</v>
@@ -8510,7 +8510,7 @@
         <v>7.7</v>
       </c>
       <c r="E264" s="6">
-        <v>231.33</v>
+        <v>236.42319578445461</v>
       </c>
       <c r="F264" s="4">
         <v>9.35E-2</v>
@@ -8537,7 +8537,7 @@
         <v>7.9</v>
       </c>
       <c r="E265" s="6">
-        <v>231.72499999999999</v>
+        <v>236.49728908307401</v>
       </c>
       <c r="F265" s="4">
         <v>7.0000000000000007E-2</v>
@@ -8564,7 +8564,7 @@
         <v>8</v>
       </c>
       <c r="E266" s="6">
-        <v>232.22900000000001</v>
+        <v>236.59164520673266</v>
       </c>
       <c r="F266" s="4">
         <v>7.4285714285714288E-2</v>
@@ -8591,7 +8591,7 @@
         <v>7.7</v>
       </c>
       <c r="E267" s="6">
-        <v>232.56899999999999</v>
+        <v>236.65518254991588</v>
       </c>
       <c r="F267" s="4">
         <v>9.8947368421052631E-2</v>
@@ -8618,7 +8618,7 @@
         <v>7.5</v>
       </c>
       <c r="E268" s="6">
-        <v>232.79400000000001</v>
+        <v>236.69717826768567</v>
       </c>
       <c r="F268" s="4">
         <v>8.6999999999999994E-2</v>
@@ -8645,7 +8645,7 @@
         <v>7.6</v>
       </c>
       <c r="E269" s="6">
-        <v>232.83199999999999</v>
+        <v>236.70426687113516</v>
       </c>
       <c r="F269" s="4">
         <v>0.06</v>
@@ -8672,7 +8672,7 @@
         <v>7.5</v>
       </c>
       <c r="E270" s="6">
-        <v>232.99600000000001</v>
+        <v>236.73484652627604</v>
       </c>
       <c r="F270" s="4">
         <v>4.409090909090909E-2</v>
@@ -8699,7 +8699,7 @@
         <v>7.5</v>
       </c>
       <c r="E271" s="6">
-        <v>233.35</v>
+        <v>236.80078052211746</v>
       </c>
       <c r="F271" s="4">
         <v>5.0500000000000003E-2</v>
@@ -8726,7 +8726,7 @@
         <v>7.3</v>
       </c>
       <c r="E272" s="6">
-        <v>233.88</v>
+        <v>236.8993085165246</v>
       </c>
       <c r="F272" s="4">
         <v>3.5454545454545454E-2</v>
@@ -8753,7 +8753,7 @@
         <v>7.2</v>
       </c>
       <c r="E273" s="6">
-        <v>234.33600000000001</v>
+        <v>236.98390124567572</v>
       </c>
       <c r="F273" s="4">
         <v>4.363636363636364E-2</v>
@@ -8780,7 +8780,7 @@
         <v>7.2</v>
       </c>
       <c r="E274" s="6">
-        <v>234.7</v>
+        <v>237.05130895985923</v>
       </c>
       <c r="F274" s="4">
         <v>1.6E-2</v>
@@ -8807,7 +8807,7 @@
         <v>7.2</v>
       </c>
       <c r="E275" s="6">
-        <v>234.92099999999999</v>
+        <v>237.09218408579514</v>
       </c>
       <c r="F275" s="4">
         <v>4.7272727272727272E-2</v>
@@ -8834,7 +8834,7 @@
         <v>6.9</v>
       </c>
       <c r="E276" s="6">
-        <v>235.35900000000001</v>
+        <v>237.17308101446525</v>
       </c>
       <c r="F276" s="4">
         <v>6.7894736842105258E-2</v>
@@ -8861,7 +8861,7 @@
         <v>6.7</v>
       </c>
       <c r="E277" s="6">
-        <v>235.75899999999999</v>
+        <v>237.24682807337803</v>
       </c>
       <c r="F277" s="4">
         <v>6.6666666666666666E-2</v>
@@ -8888,7 +8888,7 @@
         <v>6.6</v>
       </c>
       <c r="E278" s="6">
-        <v>235.96100000000001</v>
+        <v>237.28402280360217</v>
       </c>
       <c r="F278" s="4">
         <v>4.3333333333333335E-2</v>
@@ -8915,7 +8915,7 @@
         <v>6.7</v>
       </c>
       <c r="E279" s="6">
-        <v>236.185</v>
+        <v>237.32523123118398</v>
       </c>
       <c r="F279" s="4">
         <v>5.2631578947368418E-2</v>
@@ -8942,7 +8942,7 @@
         <v>6.7</v>
       </c>
       <c r="E280" s="6">
-        <v>236.625</v>
+        <v>237.40606269718532</v>
       </c>
       <c r="F280" s="4">
         <v>5.2380952380952382E-2</v>
@@ -8969,7 +8969,7 @@
         <v>6.2</v>
       </c>
       <c r="E281" s="6">
-        <v>237.072</v>
+        <v>237.48802635371354</v>
       </c>
       <c r="F281" s="4">
         <v>3.0952380952380953E-2</v>
@@ -8996,7 +8996,7 @@
         <v>6.3</v>
       </c>
       <c r="E282" s="6">
-        <v>237.529</v>
+        <v>237.57166403655506</v>
       </c>
       <c r="F282" s="4">
         <v>3.2380952380952378E-2</v>
@@ -9023,7 +9023,7 @@
         <v>6.1</v>
       </c>
       <c r="E283" s="6">
-        <v>237.83699999999999</v>
+        <v>237.62794181794632</v>
       </c>
       <c r="F283" s="4">
         <v>3.5714285714285712E-2</v>
@@ -9050,7 +9050,7 @@
         <v>6.2</v>
       </c>
       <c r="E284" s="6">
-        <v>238.19499999999999</v>
+        <v>237.69326408780759</v>
       </c>
       <c r="F284" s="4">
         <v>2.6363636363636363E-2</v>
@@ -9077,7 +9077,7 @@
         <v>6.1</v>
       </c>
       <c r="E285" s="6">
-        <v>238.405</v>
+        <v>237.73153594978905</v>
       </c>
       <c r="F285" s="4">
         <v>3.2857142857142856E-2</v>
@@ -9104,7 +9104,7 @@
         <v>5.9</v>
       </c>
       <c r="E286" s="6">
-        <v>238.786</v>
+        <v>237.80088605604232</v>
       </c>
       <c r="F286" s="4">
         <v>0.02</v>
@@ -9131,7 +9131,7 @@
         <v>5.7</v>
       </c>
       <c r="E287" s="6">
-        <v>239.191</v>
+        <v>237.87448344975135</v>
       </c>
       <c r="F287" s="4">
         <v>1.6818181818181819E-2</v>
@@ -9158,7 +9158,7 @@
         <v>5.8</v>
       </c>
       <c r="E288" s="6">
-        <v>239.458</v>
+        <v>237.92293508704518</v>
       </c>
       <c r="F288" s="4">
         <v>2.1666666666666667E-2</v>
@@ -9185,7 +9185,7 @@
         <v>5.6</v>
       </c>
       <c r="E289" s="6">
-        <v>239.584</v>
+        <v>237.94578114479447</v>
       </c>
       <c r="F289" s="4">
         <v>2.9090909090909091E-2</v>
@@ -9212,7 +9212,7 @@
         <v>5.7</v>
       </c>
       <c r="E290" s="6">
-        <v>239.81100000000001</v>
+        <v>237.98691000711477</v>
       </c>
       <c r="F290" s="4">
         <v>2.75E-2</v>
@@ -9239,7 +9239,7 @@
         <v>5.5</v>
       </c>
       <c r="E291" s="6">
-        <v>240.172</v>
+        <v>238.05223746143253</v>
       </c>
       <c r="F291" s="4">
         <v>1.7894736842105262E-2</v>
@@ -9266,7 +9266,7 @@
         <v>5.4</v>
       </c>
       <c r="E292" s="6">
-        <v>240.755</v>
+        <v>238.15753153183201</v>
       </c>
       <c r="F292" s="4">
         <v>2.7727272727272729E-2</v>
@@ -9293,7 +9293,7 @@
         <v>5.4</v>
       </c>
       <c r="E293" s="6">
-        <v>241.346</v>
+        <v>238.26401053410655</v>
       </c>
       <c r="F293" s="4">
         <v>2.3181818181818182E-2</v>
@@ -9320,7 +9320,7 @@
         <v>5.6</v>
       </c>
       <c r="E294" s="6">
-        <v>241.68799999999999</v>
+        <v>238.3255087879065</v>
       </c>
       <c r="F294" s="4">
         <v>1.6500000000000001E-2</v>
@@ -9347,7 +9347,7 @@
         <v>5.3</v>
       </c>
       <c r="E295" s="6">
-        <v>242.06399999999999</v>
+        <v>238.39302055347207</v>
       </c>
       <c r="F295" s="4">
         <v>1.4999999999999999E-2</v>
@@ -9374,7 +9374,7 @@
         <v>5.2</v>
       </c>
       <c r="E296" s="6">
-        <v>242.565</v>
+        <v>238.48281361700873</v>
       </c>
       <c r="F296" s="4">
         <v>3.2272727272727272E-2</v>
@@ -9401,7 +9401,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E297" s="6">
-        <v>242.81700000000001</v>
+        <v>238.52790891072496</v>
       </c>
       <c r="F297" s="4">
         <v>7.1904761904761902E-2</v>
@@ -9428,7 +9428,7 @@
         <v>5</v>
       </c>
       <c r="E298" s="6">
-        <v>243.316</v>
+        <v>238.61706682536231</v>
       </c>
       <c r="F298" s="4">
         <v>2.238095238095238E-2</v>
@@ -9455,7 +9455,7 @@
         <v>5</v>
       </c>
       <c r="E299" s="6">
-        <v>243.768</v>
+        <v>238.69766941635987</v>
       </c>
       <c r="F299" s="4">
         <v>1.5238095238095238E-2</v>
@@ -9482,7 +9482,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E300" s="6">
-        <v>244.24100000000001</v>
+        <v>238.78185694333865</v>
       </c>
       <c r="F300" s="4">
         <v>0.12473684210526316</v>
@@ -9509,7 +9509,7 @@
         <v>5</v>
       </c>
       <c r="E301" s="6">
-        <v>244.547</v>
+        <v>238.83623394474779</v>
       </c>
       <c r="F301" s="4">
         <v>0.22772727272727272</v>

</xml_diff>

<commit_message>
deleted:    Graphs/IRF 68.svg 	new file:   Graphs/IRF68.jpeg 	new file:   Graphs/forecast_err_variance_decomp.jpg 	new file:   Graphs/historical_decomp_nolegend.jpg 	modified:   JessicaCremonese_AM_Project.aux 	modified:   JessicaCremonese_AM_Project.log 	modified:   JessicaCremonese_AM_Project.pdf 	modified:   JessicaCremonese_AM_Project.synctex.gz 	modified:   JessicaCremonese_AM_Project.tex 	modified:   database_mpshocks_infoshocks.xlsx 	modified:   draft_definitive_code_AM_efrem.m
</commit_message>
<xml_diff>
--- a/database_mpshocks_infoshocks.xlsx
+++ b/database_mpshocks_infoshocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Desktop\AppMacro_Project_Efrem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99D93CE-650B-42D0-86BC-788E0E58D55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03210F87-E804-410C-8C6E-6F284DF2E082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
+    <workbookView xWindow="8388" yWindow="2640" windowWidth="14652" windowHeight="9600" xr2:uid="{7F14BA07-F3DD-4C2F-A99A-BC5AD2C8E3ED}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1381,7 +1381,7 @@
   <dimension ref="A1:Q302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I2" sqref="I2:I301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,10 +1389,10 @@
     <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="143" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>